<commit_message>
Added new devices to list
</commit_message>
<xml_diff>
--- a/android/Script_tested_devices.xlsx
+++ b/android/Script_tested_devices.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Compatiblity list Live Script</t>
   </si>
@@ -47,6 +47,39 @@
 Chipset not possible
 Logcat command not usable with -S and -b
 Settings commands not usable with option list</t>
+  </si>
+  <si>
+    <t>SM-G920F</t>
+  </si>
+  <si>
+    <t>Android 7</t>
+  </si>
+  <si>
+    <t>WIFI MAC not possible</t>
+  </si>
+  <si>
+    <t>Motorala</t>
+  </si>
+  <si>
+    <t>Android 9</t>
+  </si>
+  <si>
+    <t>XT-1925-5</t>
+  </si>
+  <si>
+    <t>Model Name</t>
+  </si>
+  <si>
+    <t>Galaxy S6</t>
+  </si>
+  <si>
+    <t>moto g6</t>
+  </si>
+  <si>
+    <t>Galaxy Tab 3</t>
+  </si>
+  <si>
+    <t>Everythings works</t>
   </si>
 </sst>
 </file>
@@ -388,25 +421,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5703125" customWidth="1"/>
-    <col min="4" max="4" width="45" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -414,13 +448,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -428,10 +465,47 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added newly tested devices
</commit_message>
<xml_diff>
--- a/android/Script_tested_devices.xlsx
+++ b/android/Script_tested_devices.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$4:$E$4</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>Compatiblity list Live Script</t>
   </si>
@@ -58,9 +61,6 @@
     <t>WIFI MAC not possible</t>
   </si>
   <si>
-    <t>Motorala</t>
-  </si>
-  <si>
     <t>Android 9</t>
   </si>
   <si>
@@ -80,6 +80,25 @@
   </si>
   <si>
     <t>Everythings works</t>
+  </si>
+  <si>
+    <t>Motorola</t>
+  </si>
+  <si>
+    <t>Huawei</t>
+  </si>
+  <si>
+    <t>ALE-L21</t>
+  </si>
+  <si>
+    <t>P8 Lite</t>
+  </si>
+  <si>
+    <t>Android 6</t>
+  </si>
+  <si>
+    <t>WIFI MAC not possible
+Serial Number not possible</t>
   </si>
 </sst>
 </file>
@@ -421,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
@@ -448,7 +467,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -465,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -482,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -493,22 +512,40 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A4:E4"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
New Script for Freenet app Android
</commit_message>
<xml_diff>
--- a/android/Script_tested_devices.xlsx
+++ b/android/Script_tested_devices.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Compatiblity list Live Script</t>
   </si>
@@ -123,6 +123,18 @@
   </si>
   <si>
     <t>Logcat added without option flags</t>
+  </si>
+  <si>
+    <t>Wiko</t>
+  </si>
+  <si>
+    <t>Sunny3</t>
+  </si>
+  <si>
+    <t>Android 8.1.0</t>
+  </si>
+  <si>
+    <t>W_K120</t>
   </si>
 </sst>
 </file>
@@ -464,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +616,23 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>